<commit_message>
Add files of testing for Rudhra development, also add my part on document "Interaction 2 Plan".
</commit_message>
<xml_diff>
--- a/Documentation/Task List -Iteration 2 - Epworth Project .xlsx
+++ b/Documentation/Task List -Iteration 2 - Epworth Project .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="580" windowWidth="11180" windowHeight="7880" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
@@ -2516,6 +2516,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1701800</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 5" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2838,6 +2889,57 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="Rectangle 5" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 5" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3230,6 +3332,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9664700</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 5" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3552,6 +3705,57 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="Rectangle 5" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2286000</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 5" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3944,6 +4148,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2286000</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 5" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6170,8 +6425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added all my individual and group submition files.
</commit_message>
<xml_diff>
--- a/Documentation/Task List -Iteration 2 - Epworth Project .xlsx
+++ b/Documentation/Task List -Iteration 2 - Epworth Project .xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="570" windowWidth="11175" windowHeight="7875" activeTab="1"/>
+    <workbookView xWindow="400" yWindow="580" windowWidth="38000" windowHeight="21920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,12 @@
     <sheet name="Iteration 4" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration 5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -339,7 +344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="378">
   <si>
     <t>Team Name</t>
   </si>
@@ -1479,7 +1484,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="47" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1698,6 +1703,18 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2034,10 +2051,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2186,8 +2207,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2632,6 +2660,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1701800</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 5" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3064,6 +3143,57 @@
           <a:tailEnd/>
         </a:ln>
       </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9639300</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -3502,6 +3632,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9664700</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 5" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3934,6 +4115,57 @@
           <a:tailEnd/>
         </a:ln>
       </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2286000</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 5" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -4372,6 +4604,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2286000</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 5" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4668,21 +4951,21 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
-    <col min="3" max="3" width="102.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
-    <col min="9" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" customWidth="1"/>
+    <col min="3" max="3" width="102.5" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="16" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="21" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4701,7 +4984,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="24" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -4724,7 +5007,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="24" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="45" t="s">
         <v>371</v>
@@ -4745,7 +5028,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="9.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -4764,7 +5047,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="22.5" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>2</v>
@@ -4787,7 +5070,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="22.5" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>3</v>
@@ -4810,7 +5093,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="22.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -4833,7 +5116,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="12.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4852,7 +5135,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
         <v>5</v>
@@ -4873,7 +5156,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="13.5" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4892,7 +5175,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="33.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="6" t="s">
         <v>6</v>
@@ -4923,7 +5206,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="30.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="7" t="s">
         <v>12</v>
@@ -4951,7 +5234,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="30" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="s">
@@ -4977,7 +5260,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="15" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="s">
@@ -5000,7 +5283,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="30" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
@@ -5024,7 +5307,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="7" t="s">
         <v>20</v>
@@ -5049,7 +5332,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="30" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="7" t="s">
         <v>23</v>
@@ -5075,7 +5358,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="s">
@@ -5098,7 +5381,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="7" t="s">
         <v>27</v>
@@ -5124,7 +5407,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="30" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8" t="s">
@@ -5148,7 +5431,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="15" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8" t="s">
@@ -5172,7 +5455,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="15" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8" t="s">
@@ -5196,7 +5479,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="15" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="7" t="s">
         <v>32</v>
@@ -5222,7 +5505,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="15" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8" t="s">
@@ -5246,7 +5529,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="30" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8" t="s">
@@ -5270,7 +5553,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="18" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="7" t="s">
         <v>36</v>
@@ -5296,7 +5579,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="18" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8" t="s">
@@ -5320,7 +5603,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="18" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8" t="s">
@@ -5344,7 +5627,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="18" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8" t="s">
@@ -5368,7 +5651,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="15" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8" t="s">
@@ -5392,7 +5675,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="15.75" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="13" t="s">
         <v>42</v>
@@ -5417,7 +5700,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="13.5" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -5436,7 +5719,7 @@
       <c r="P32" s="17"/>
       <c r="Q32" s="17"/>
     </row>
-    <row r="33" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="12.75" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -5455,7 +5738,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="12.75" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -5474,7 +5757,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="12.75" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -5493,7 +5776,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="12.75" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
         <v>45</v>
@@ -5514,7 +5797,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="12.75" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="10"/>
@@ -5533,7 +5816,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="12.75" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>46</v>
@@ -5554,7 +5837,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="12.75" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
         <v>47</v>
@@ -5575,7 +5858,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="12.75" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="18" t="e">
         <f>D19</f>
@@ -5597,7 +5880,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="12.75" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>48</v>
@@ -5618,7 +5901,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="12.75" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="10"/>
@@ -5637,7 +5920,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="12.75" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="10"/>
@@ -5656,7 +5939,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="12.75" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="10"/>
@@ -5675,7 +5958,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="12.75" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="10"/>
@@ -5694,7 +5977,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="12.75" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="10"/>
@@ -5713,7 +5996,7 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="12.75" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="10"/>
@@ -5732,7 +6015,7 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="12.75" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="10"/>
@@ -5751,7 +6034,7 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" ht="12.75" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="10"/>
@@ -5770,7 +6053,7 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" ht="12.75" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="10"/>
@@ -5789,7 +6072,7 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" ht="12.75" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -5808,7 +6091,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" ht="12.75" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="2" t="s">
         <v>49</v>
@@ -5829,7 +6112,7 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" ht="12.75" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
@@ -5848,7 +6131,7 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
     </row>
-    <row r="54" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="12.75" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
         <v>50</v>
@@ -5869,7 +6152,7 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
     </row>
-    <row r="55" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" ht="12.75" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
         <v>51</v>
@@ -5890,7 +6173,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
     </row>
-    <row r="56" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" ht="12.75" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="18" t="str">
         <f>D20</f>
@@ -5912,7 +6195,7 @@
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
     </row>
-    <row r="57" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" ht="12.75" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
         <v>52</v>
@@ -5933,7 +6216,7 @@
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
     </row>
-    <row r="58" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" ht="12.75" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="10"/>
@@ -5952,7 +6235,7 @@
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
     </row>
-    <row r="59" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" ht="12.75" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="10"/>
@@ -5971,7 +6254,7 @@
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
     </row>
-    <row r="60" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" ht="12.75" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="10"/>
@@ -5990,7 +6273,7 @@
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
     </row>
-    <row r="61" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="12.75" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="10"/>
@@ -6009,7 +6292,7 @@
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
     </row>
-    <row r="62" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" ht="12.75" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="10"/>
@@ -6028,7 +6311,7 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" ht="12.75" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="10"/>
@@ -6047,7 +6330,7 @@
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
     </row>
-    <row r="64" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" ht="12.75" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="10"/>
@@ -6066,7 +6349,7 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
     </row>
-    <row r="65" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" ht="12.75" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="10"/>
@@ -6085,7 +6368,7 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" ht="12.75" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="10"/>
@@ -6104,7 +6387,7 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" ht="12.75" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -6123,7 +6406,7 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" ht="12.75" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="2" t="s">
         <v>53</v>
@@ -6144,7 +6427,7 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" ht="12.75" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="10"/>
@@ -6163,7 +6446,7 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" ht="12.75" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="1" t="s">
         <v>54</v>
@@ -6184,7 +6467,7 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
     </row>
-    <row r="71" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" ht="12.75" customHeight="1">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
         <v>55</v>
@@ -6205,7 +6488,7 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
     </row>
-    <row r="72" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" ht="12.75" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="18" t="str">
         <f>D21</f>
@@ -6227,7 +6510,7 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" ht="12.75" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
         <v>56</v>
@@ -6248,7 +6531,7 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" ht="12.75" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="10"/>
@@ -6267,7 +6550,7 @@
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
     </row>
-    <row r="75" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" ht="12.75" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="10"/>
@@ -6286,7 +6569,7 @@
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
     </row>
-    <row r="76" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" ht="12.75" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="10"/>
@@ -6305,7 +6588,7 @@
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
     </row>
-    <row r="77" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" ht="12.75" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="10"/>
@@ -6324,7 +6607,7 @@
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
     </row>
-    <row r="78" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" ht="12.75" customHeight="1">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="10"/>
@@ -6343,7 +6626,7 @@
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
     </row>
-    <row r="79" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" ht="12.75" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="10"/>
@@ -6362,7 +6645,7 @@
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
     </row>
-    <row r="80" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" ht="12.75" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="10"/>
@@ -6381,7 +6664,7 @@
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
     </row>
-    <row r="81" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" ht="12.75" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="10"/>
@@ -6400,7 +6683,7 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
     </row>
-    <row r="82" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" ht="12.75" customHeight="1">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="10"/>
@@ -6419,7 +6702,7 @@
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
     </row>
-    <row r="83" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" ht="12.75" customHeight="1">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -6438,7 +6721,7 @@
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
     </row>
-    <row r="84" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" ht="12.75" customHeight="1">
       <c r="A84" s="1"/>
       <c r="B84" s="2" t="s">
         <v>57</v>
@@ -6459,7 +6742,7 @@
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
     </row>
-    <row r="85" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" ht="12.75" customHeight="1">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="10"/>
@@ -6478,7 +6761,7 @@
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
     </row>
-    <row r="86" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" ht="12.75" customHeight="1">
       <c r="A86" s="1"/>
       <c r="B86" s="1" t="s">
         <v>58</v>
@@ -6499,7 +6782,7 @@
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
     </row>
-    <row r="87" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" ht="12.75" customHeight="1">
       <c r="A87" s="1"/>
       <c r="B87" s="1" t="s">
         <v>59</v>
@@ -6520,7 +6803,7 @@
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
     </row>
-    <row r="88" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" ht="12.75" customHeight="1">
       <c r="A88" s="1"/>
       <c r="B88" s="18" t="str">
         <f>D22</f>
@@ -6542,7 +6825,7 @@
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
     </row>
-    <row r="89" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" ht="12.75" customHeight="1">
       <c r="A89" s="1"/>
       <c r="B89" s="1" t="s">
         <v>60</v>
@@ -6563,7 +6846,7 @@
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
     </row>
-    <row r="90" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" ht="12.75" customHeight="1">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="10"/>
@@ -6586,6 +6869,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6593,25 +6881,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="141.140625" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
-    <col min="9" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="141.1640625" customWidth="1"/>
+    <col min="4" max="4" width="43.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="16" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -6630,7 +6918,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="23.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>61</v>
@@ -6653,7 +6941,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="20" t="str">
         <f>'Iteration 1'!B3</f>
@@ -6677,7 +6965,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="9" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -6696,7 +6984,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="23.25" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="str">
         <f>'Iteration 1'!B5</f>
@@ -6720,7 +7008,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="23.25" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="str">
         <f>'Iteration 1'!B6</f>
@@ -6744,7 +7032,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="23.25" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="str">
         <f>'Iteration 1'!B7</f>
@@ -6768,7 +7056,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6787,7 +7075,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
         <v>66</v>
@@ -6808,7 +7096,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="13.5" customHeight="1" thickBot="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -6827,7 +7115,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="1"/>
       <c r="B11" s="22" t="s">
         <v>67</v>
@@ -6864,7 +7152,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="15.75" customHeight="1" thickTop="1">
       <c r="A12" s="1"/>
       <c r="B12" s="7" t="s">
         <v>73</v>
@@ -6896,7 +7184,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="15" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="s">
@@ -6922,7 +7210,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="17.25" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="s">
@@ -6946,7 +7234,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
@@ -6976,7 +7264,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="18.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
@@ -7000,7 +7288,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
@@ -7024,7 +7312,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="s">
@@ -7047,7 +7335,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="7" t="s">
         <v>87</v>
@@ -7073,7 +7361,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8" t="s">
@@ -7097,7 +7385,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="15" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="7" t="s">
         <v>90</v>
@@ -7124,7 +7412,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="15" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="7"/>
       <c r="C22" s="28" t="s">
@@ -7149,7 +7437,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="15" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="7" t="s">
         <v>95</v>
@@ -7177,7 +7465,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="15" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8" t="s">
@@ -7207,7 +7495,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="15" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8" t="s">
@@ -7237,7 +7525,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="15" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8" t="s">
@@ -7267,7 +7555,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="15" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8" t="s">
@@ -7282,7 +7570,9 @@
       <c r="F27" s="25"/>
       <c r="G27" s="25"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="25"/>
+      <c r="I27" s="46" t="s">
+        <v>376</v>
+      </c>
       <c r="J27" s="46" t="s">
         <v>377</v>
       </c>
@@ -7296,7 +7586,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="15" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="7"/>
       <c r="C28" s="30" t="s">
@@ -7320,7 +7610,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="13.5" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="7"/>
       <c r="C29" s="31" t="s">
@@ -7344,7 +7634,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="15" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="7" t="s">
         <v>109</v>
@@ -7376,7 +7666,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="15" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8" t="s">
@@ -7389,7 +7679,7 @@
       <c r="E31" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F31" s="25"/>
+      <c r="F31" s="50"/>
       <c r="G31" s="25"/>
       <c r="H31" s="1"/>
       <c r="I31" s="25"/>
@@ -7402,7 +7692,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="15" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8" t="s">
@@ -7434,7 +7724,7 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="15" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8" t="s">
@@ -7462,7 +7752,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="15" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8" t="s">
@@ -7490,7 +7780,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="15.75" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="7"/>
       <c r="C35" s="14"/>
@@ -7509,7 +7799,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="13.5" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -7528,7 +7818,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="12.75" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -7547,7 +7837,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="12.75" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="2" t="s">
         <v>116</v>
@@ -7570,7 +7860,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="12.75" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="10" t="s">
@@ -7591,7 +7881,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="12.75" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>119</v>
@@ -7614,7 +7904,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="12.75" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>121</v>
@@ -7637,7 +7927,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="12.75" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="18" t="str">
         <f>D19</f>
@@ -7661,7 +7951,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="12.75" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>124</v>
@@ -7684,7 +7974,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="12.75" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="10" t="s">
@@ -7705,7 +7995,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="12.75" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="10" t="s">
@@ -7726,7 +8016,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="12.75" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="10"/>
@@ -7745,7 +8035,7 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="12.75" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="10"/>
@@ -7764,7 +8054,7 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="12.75" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="10"/>
@@ -7783,7 +8073,7 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" ht="12.75" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="10"/>
@@ -7802,7 +8092,7 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" ht="12.75" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="10"/>
@@ -7821,7 +8111,7 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" ht="12.75" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="10"/>
@@ -7840,7 +8130,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" ht="12.75" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="10"/>
@@ -7859,7 +8149,7 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" ht="12.75" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
@@ -7878,7 +8168,7 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
     </row>
-    <row r="54" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="12.75" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="10"/>
@@ -7897,7 +8187,7 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
     </row>
-    <row r="55" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" ht="12.75" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="10"/>
@@ -7916,7 +8206,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
     </row>
-    <row r="56" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" ht="12.75" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="10"/>
@@ -7935,7 +8225,7 @@
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
     </row>
-    <row r="57" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" ht="12.75" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -7954,7 +8244,7 @@
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
     </row>
-    <row r="58" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" ht="12.75" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>128</v>
       </c>
@@ -7983,7 +8273,7 @@
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
     </row>
-    <row r="59" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" ht="12.75" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="10"/>
@@ -8002,7 +8292,7 @@
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
     </row>
-    <row r="60" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" ht="12.75" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
         <v>133</v>
@@ -8029,7 +8319,7 @@
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
     </row>
-    <row r="61" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="12.75" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
         <v>135</v>
@@ -8056,7 +8346,7 @@
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
     </row>
-    <row r="62" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" ht="12.75" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="18" t="str">
         <f>D24</f>
@@ -8084,7 +8374,7 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" ht="12.75" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
         <v>138</v>
@@ -8111,7 +8401,7 @@
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
     </row>
-    <row r="64" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" ht="12.75" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="10" t="s">
@@ -8136,7 +8426,7 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
     </row>
-    <row r="65" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" ht="12.75" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="10" t="s">
@@ -8161,7 +8451,7 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" ht="12.75" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="10" t="s">
@@ -8186,7 +8476,7 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" ht="12.75" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="10"/>
@@ -8205,7 +8495,7 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" ht="12.75" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="10"/>
@@ -8229,7 +8519,7 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" ht="12.75" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -8248,7 +8538,7 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" ht="12.75" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="18" t="s">
         <v>144</v>
@@ -8275,7 +8565,7 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
     </row>
-    <row r="71" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" ht="12.75" customHeight="1">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="10"/>
@@ -8294,7 +8584,7 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
     </row>
-    <row r="72" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" ht="12.75" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="1" t="s">
         <v>148</v>
@@ -8321,7 +8611,7 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" ht="12.75" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
         <v>150</v>
@@ -8348,7 +8638,7 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" ht="12.75" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="18" t="str">
         <f>D25</f>
@@ -8376,7 +8666,7 @@
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
     </row>
-    <row r="75" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" ht="12.75" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
         <v>153</v>
@@ -8403,7 +8693,7 @@
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
     </row>
-    <row r="76" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" ht="12.75" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="10"/>
@@ -8422,7 +8712,7 @@
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
     </row>
-    <row r="77" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" ht="12.75" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="10"/>
@@ -8441,7 +8731,7 @@
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
     </row>
-    <row r="78" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" ht="12.75" customHeight="1">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="10"/>
@@ -8460,7 +8750,7 @@
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
     </row>
-    <row r="79" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" ht="12.75" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="10"/>
@@ -8479,7 +8769,7 @@
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
     </row>
-    <row r="80" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" ht="12.75" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="10"/>
@@ -8503,7 +8793,7 @@
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
     </row>
-    <row r="81" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" ht="12.75" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -8522,7 +8812,7 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
     </row>
-    <row r="82" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" ht="12.75" customHeight="1">
       <c r="A82" s="1"/>
       <c r="B82" s="18" t="s">
         <v>156</v>
@@ -8549,7 +8839,7 @@
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
     </row>
-    <row r="83" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" ht="12.75" customHeight="1">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="10" t="s">
@@ -8574,7 +8864,7 @@
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
     </row>
-    <row r="84" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" ht="12.75" customHeight="1">
       <c r="A84" s="1"/>
       <c r="B84" s="1" t="s">
         <v>161</v>
@@ -8601,7 +8891,7 @@
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
     </row>
-    <row r="85" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" ht="12.75" customHeight="1">
       <c r="A85" s="1"/>
       <c r="B85" s="1" t="s">
         <v>163</v>
@@ -8628,7 +8918,7 @@
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
     </row>
-    <row r="86" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" ht="12.75" customHeight="1">
       <c r="A86" s="1"/>
       <c r="B86" s="18" t="str">
         <f>D26</f>
@@ -8656,7 +8946,7 @@
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
     </row>
-    <row r="87" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" ht="12.75" customHeight="1">
       <c r="A87" s="1"/>
       <c r="B87" s="1" t="s">
         <v>166</v>
@@ -8683,7 +8973,7 @@
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
     </row>
-    <row r="88" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" ht="12.75" customHeight="1">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="10"/>
@@ -8702,7 +8992,7 @@
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
     </row>
-    <row r="89" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" ht="12.75" customHeight="1">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="10"/>
@@ -8721,7 +9011,7 @@
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
     </row>
-    <row r="90" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" ht="12.75" customHeight="1">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="10"/>
@@ -8740,7 +9030,7 @@
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
     </row>
-    <row r="91" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" ht="12.75" customHeight="1">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="10"/>
@@ -8759,7 +9049,7 @@
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
     </row>
-    <row r="92" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" ht="12.75" customHeight="1">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="10"/>
@@ -8785,9 +9075,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8799,21 +9094,21 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="141.140625" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
-    <col min="9" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="3" max="3" width="141.1640625" customWidth="1"/>
+    <col min="4" max="4" width="43.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="16" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -8832,7 +9127,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="23.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>169</v>
@@ -8855,7 +9150,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="20" t="str">
         <f>'Iteration 1'!B3</f>
@@ -8877,7 +9172,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="9.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -8896,7 +9191,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="23.25" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="str">
         <f>'Iteration 1'!B5</f>
@@ -8921,7 +9216,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="23.25" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="str">
         <f>'Iteration 1'!B6</f>
@@ -8946,7 +9241,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="23.25" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="str">
         <f>'Iteration 1'!B7</f>
@@ -8971,7 +9266,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="17.25" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -8990,7 +9285,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
         <v>171</v>
@@ -9011,7 +9306,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="13.5" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -9030,7 +9325,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="16.5" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="22" t="s">
         <v>172</v>
@@ -9061,7 +9356,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="7" t="s">
         <v>178</v>
@@ -9089,7 +9384,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="15" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="s">
@@ -9115,7 +9410,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="17.25" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="s">
@@ -9139,7 +9434,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
@@ -9163,7 +9458,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="18.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
@@ -9189,7 +9484,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
@@ -9213,7 +9508,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="s">
@@ -9236,7 +9531,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="7" t="s">
         <v>190</v>
@@ -9262,7 +9557,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8" t="s">
@@ -9286,7 +9581,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="15" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="7" t="s">
         <v>193</v>
@@ -9311,7 +9606,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="15" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="7"/>
       <c r="C22" s="28" t="s">
@@ -9334,7 +9629,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="15" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="7" t="s">
         <v>198</v>
@@ -9362,7 +9657,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="15" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8" t="s">
@@ -9385,7 +9680,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="15" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8" t="s">
@@ -9411,7 +9706,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="15" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8" t="s">
@@ -9437,7 +9732,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="15" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8" t="s">
@@ -9463,7 +9758,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="15" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8" t="s">
@@ -9488,7 +9783,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="15" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="7"/>
       <c r="C29" s="30" t="s">
@@ -9512,7 +9807,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="13.5" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="7"/>
       <c r="C30" s="31" t="s">
@@ -9536,7 +9831,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="15" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="7" t="s">
         <v>214</v>
@@ -9564,7 +9859,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="15" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8" t="s">
@@ -9590,7 +9885,7 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="15" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8" t="s">
@@ -9616,7 +9911,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="15" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8" t="s">
@@ -9639,7 +9934,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="15" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
@@ -9663,7 +9958,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="15" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8" t="s">
@@ -9687,7 +9982,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="15.75" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="7"/>
       <c r="C37" s="14"/>
@@ -9706,7 +10001,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="13.5" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -9725,7 +10020,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="12.75" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -9744,7 +10039,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="12.75" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
         <v>225</v>
@@ -9765,7 +10060,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="12.75" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="10"/>
@@ -9784,7 +10079,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="12.75" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>226</v>
@@ -9805,7 +10100,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="12.75" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>227</v>
@@ -9826,7 +10121,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="12.75" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="18" t="str">
         <f>D19</f>
@@ -9848,7 +10143,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="12.75" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>228</v>
@@ -9869,7 +10164,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="12.75" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="10"/>
@@ -9888,7 +10183,7 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="12.75" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="10"/>
@@ -9907,7 +10202,7 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="12.75" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="10"/>
@@ -9926,7 +10221,7 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" ht="12.75" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="10"/>
@@ -9945,7 +10240,7 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" ht="12.75" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="10"/>
@@ -9964,7 +10259,7 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" ht="12.75" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="10"/>
@@ -9983,7 +10278,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" ht="12.75" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="10"/>
@@ -10002,7 +10297,7 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" ht="12.75" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
@@ -10021,7 +10316,7 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
     </row>
-    <row r="54" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="12.75" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="10"/>
@@ -10040,7 +10335,7 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
     </row>
-    <row r="55" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" ht="12.75" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="10"/>
@@ -10059,7 +10354,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
     </row>
-    <row r="56" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" ht="12.75" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="10"/>
@@ -10078,7 +10373,7 @@
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
     </row>
-    <row r="57" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" ht="12.75" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="10"/>
@@ -10097,7 +10392,7 @@
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
     </row>
-    <row r="58" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" ht="12.75" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="10"/>
@@ -10116,7 +10411,7 @@
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
     </row>
-    <row r="59" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" ht="12.75" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -10135,7 +10430,7 @@
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
     </row>
-    <row r="60" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" ht="12.75" customHeight="1">
       <c r="A60" s="1" t="s">
         <v>229</v>
       </c>
@@ -10164,7 +10459,7 @@
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
     </row>
-    <row r="61" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="12.75" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="10"/>
@@ -10183,7 +10478,7 @@
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
     </row>
-    <row r="62" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" ht="12.75" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
         <v>234</v>
@@ -10212,7 +10507,7 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" ht="12.75" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
         <v>237</v>
@@ -10239,7 +10534,7 @@
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
     </row>
-    <row r="64" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" ht="12.75" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="18" t="str">
         <f>D25</f>
@@ -10267,7 +10562,7 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
     </row>
-    <row r="65" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" ht="12.75" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
         <v>240</v>
@@ -10294,7 +10589,7 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" ht="12.75" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="10"/>
@@ -10313,7 +10608,7 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" ht="12.75" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="10"/>
@@ -10332,7 +10627,7 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" ht="12.75" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="10"/>
@@ -10351,7 +10646,7 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" ht="12.75" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="10"/>
@@ -10370,7 +10665,7 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" ht="12.75" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="10"/>
@@ -10394,7 +10689,7 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
     </row>
-    <row r="71" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" ht="12.75" customHeight="1">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -10413,7 +10708,7 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
     </row>
-    <row r="72" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" ht="12.75" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="18" t="s">
         <v>243</v>
@@ -10440,7 +10735,7 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" ht="12.75" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="10"/>
@@ -10459,7 +10754,7 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" ht="12.75" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="1" t="s">
         <v>247</v>
@@ -10480,7 +10775,7 @@
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
     </row>
-    <row r="75" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" ht="12.75" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
         <v>248</v>
@@ -10501,7 +10796,7 @@
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
     </row>
-    <row r="76" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" ht="12.75" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="18" t="str">
         <f>D26</f>
@@ -10523,7 +10818,7 @@
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
     </row>
-    <row r="77" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" ht="12.75" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1" t="s">
         <v>249</v>
@@ -10544,7 +10839,7 @@
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
     </row>
-    <row r="78" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" ht="12.75" customHeight="1">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="10"/>
@@ -10563,7 +10858,7 @@
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
     </row>
-    <row r="79" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" ht="12.75" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="10"/>
@@ -10582,7 +10877,7 @@
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
     </row>
-    <row r="80" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" ht="12.75" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="10"/>
@@ -10601,7 +10896,7 @@
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
     </row>
-    <row r="81" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" ht="12.75" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="10"/>
@@ -10620,7 +10915,7 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
     </row>
-    <row r="82" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" ht="12.75" customHeight="1">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="10"/>
@@ -10644,7 +10939,7 @@
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
     </row>
-    <row r="83" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" ht="12.75" customHeight="1">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -10663,7 +10958,7 @@
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
     </row>
-    <row r="84" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" ht="12.75" customHeight="1">
       <c r="A84" s="1"/>
       <c r="B84" s="18" t="s">
         <v>251</v>
@@ -10690,7 +10985,7 @@
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
     </row>
-    <row r="85" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" ht="12.75" customHeight="1">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="10"/>
@@ -10709,7 +11004,7 @@
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
     </row>
-    <row r="86" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" ht="12.75" customHeight="1">
       <c r="A86" s="1"/>
       <c r="B86" s="1" t="s">
         <v>255</v>
@@ -10730,7 +11025,7 @@
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
     </row>
-    <row r="87" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" ht="12.75" customHeight="1">
       <c r="A87" s="1"/>
       <c r="B87" s="1" t="s">
         <v>256</v>
@@ -10751,7 +11046,7 @@
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
     </row>
-    <row r="88" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" ht="12.75" customHeight="1">
       <c r="A88" s="1"/>
       <c r="B88" s="18" t="str">
         <f>D27</f>
@@ -10773,7 +11068,7 @@
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
     </row>
-    <row r="89" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" ht="12.75" customHeight="1">
       <c r="A89" s="1"/>
       <c r="B89" s="1" t="s">
         <v>257</v>
@@ -10794,7 +11089,7 @@
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
     </row>
-    <row r="90" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" ht="12.75" customHeight="1">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="10"/>
@@ -10813,7 +11108,7 @@
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
     </row>
-    <row r="91" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" ht="12.75" customHeight="1">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="10"/>
@@ -10832,7 +11127,7 @@
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
     </row>
-    <row r="92" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" ht="12.75" customHeight="1">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="10"/>
@@ -10851,7 +11146,7 @@
       <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
     </row>
-    <row r="93" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" ht="12.75" customHeight="1">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="10"/>
@@ -10870,7 +11165,7 @@
       <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
     </row>
-    <row r="94" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" ht="12.75" customHeight="1">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="10"/>
@@ -10898,6 +11193,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10909,21 +11209,21 @@
       <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="3" width="95.85546875" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
-    <col min="9" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" customWidth="1"/>
+    <col min="3" max="3" width="95.83203125" customWidth="1"/>
+    <col min="4" max="4" width="43.5" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="16" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -10942,7 +11242,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="23.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>259</v>
@@ -10965,7 +11265,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="20" t="str">
         <f>'Iteration 1'!B3</f>
@@ -10987,7 +11287,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="9.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -11006,7 +11306,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="23.25" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="str">
         <f>'Iteration 1'!B5</f>
@@ -11031,7 +11331,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="23.25" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="str">
         <f>'Iteration 1'!B6</f>
@@ -11056,7 +11356,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="22.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="str">
         <f>'Iteration 1'!B7</f>
@@ -11081,7 +11381,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="12.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -11100,7 +11400,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
         <v>261</v>
@@ -11121,7 +11421,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="13.5" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -11140,7 +11440,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="16.5" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="39" t="s">
         <v>262</v>
@@ -11171,7 +11471,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="7" t="s">
         <v>268</v>
@@ -11199,7 +11499,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="15" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="s">
@@ -11225,7 +11525,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="17.25" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="s">
@@ -11249,7 +11549,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="15" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
@@ -11273,7 +11573,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
@@ -11299,7 +11599,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
@@ -11323,7 +11623,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="40" t="s">
         <v>278</v>
@@ -11350,7 +11650,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="40"/>
       <c r="C19" s="8" t="s">
@@ -11376,7 +11676,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="40"/>
       <c r="C20" s="8" t="s">
@@ -11402,7 +11702,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="15" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="40"/>
       <c r="C21" s="8" t="s">
@@ -11428,7 +11728,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="15" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="40"/>
       <c r="C22" s="30" t="s">
@@ -11452,7 +11752,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="15" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="40"/>
       <c r="C23" s="30" t="s">
@@ -11476,7 +11776,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="15" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="40"/>
       <c r="C24" s="30" t="s">
@@ -11501,7 +11801,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="15" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="40" t="s">
         <v>293</v>
@@ -11529,7 +11829,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="15" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="40"/>
       <c r="C26" s="30" t="s">
@@ -11555,7 +11855,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="12.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="41" t="s">
         <v>298</v>
@@ -11582,7 +11882,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="12.75" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="7"/>
       <c r="C28" s="31" t="s">
@@ -11608,7 +11908,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="12.75" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="7"/>
       <c r="C29" s="31" t="s">
@@ -11634,7 +11934,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="12.75" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="7"/>
       <c r="C30" s="31" t="s">
@@ -11658,7 +11958,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="13.5" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="7"/>
       <c r="C31" s="31" t="s">
@@ -11684,7 +11984,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="13.5" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="7"/>
       <c r="C32" s="31" t="s">
@@ -11708,7 +12008,7 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="15" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="40" t="s">
         <v>310</v>
@@ -11735,7 +12035,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="15" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="40" t="s">
         <v>314</v>
@@ -11763,7 +12063,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="15" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="40"/>
       <c r="C35" s="30" t="s">
@@ -11789,7 +12089,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="15" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="40"/>
       <c r="C36" s="8" t="s">
@@ -11815,7 +12115,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="15" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="40"/>
       <c r="C37" s="8" t="s">
@@ -11839,7 +12139,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="15.75" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="42" t="s">
         <v>322</v>
@@ -11864,7 +12164,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="13.5" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -11883,7 +12183,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="12.75" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -11902,7 +12202,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="12.75" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -11921,7 +12221,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="12.75" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
         <v>325</v>
@@ -11942,7 +12242,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="12.75" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="10"/>
@@ -11961,7 +12261,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="12.75" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
         <v>326</v>
@@ -11982,7 +12282,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="12.75" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>327</v>
@@ -12003,7 +12303,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="12.75" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="18" t="str">
         <f>D34</f>
@@ -12025,7 +12325,7 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="12.75" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
         <v>328</v>
@@ -12046,7 +12346,7 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="12.75" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="10"/>
@@ -12065,7 +12365,7 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" ht="12.75" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="10"/>
@@ -12084,7 +12384,7 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" ht="12.75" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="10"/>
@@ -12103,7 +12403,7 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" ht="12.75" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="10"/>
@@ -12122,7 +12422,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" ht="12.75" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="10"/>
@@ -12141,7 +12441,7 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" ht="12.75" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
@@ -12160,7 +12460,7 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
     </row>
-    <row r="54" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="12.75" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="10"/>
@@ -12179,7 +12479,7 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
     </row>
-    <row r="55" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" ht="12.75" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="10"/>
@@ -12198,7 +12498,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
     </row>
-    <row r="56" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" ht="12.75" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="10"/>
@@ -12217,7 +12517,7 @@
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
     </row>
-    <row r="57" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" ht="12.75" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="10"/>
@@ -12236,7 +12536,7 @@
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
     </row>
-    <row r="58" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" ht="12.75" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="10"/>
@@ -12255,7 +12555,7 @@
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
     </row>
-    <row r="59" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" ht="12.75" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="10"/>
@@ -12274,7 +12574,7 @@
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
     </row>
-    <row r="60" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" ht="12.75" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="10"/>
@@ -12293,7 +12593,7 @@
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
     </row>
-    <row r="61" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="12.75" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="10"/>
@@ -12312,7 +12612,7 @@
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
     </row>
-    <row r="62" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" ht="12.75" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="10"/>
@@ -12331,7 +12631,7 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" ht="12.75" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="10"/>
@@ -12350,7 +12650,7 @@
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
     </row>
-    <row r="64" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" ht="12.75" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="10"/>
@@ -12369,7 +12669,7 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
     </row>
-    <row r="65" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" ht="12.75" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="10"/>
@@ -12388,7 +12688,7 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" ht="12.75" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="10"/>
@@ -12407,7 +12707,7 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" ht="12.75" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="10"/>
@@ -12426,7 +12726,7 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" ht="12.75" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="10"/>
@@ -12445,7 +12745,7 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" ht="12.75" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="10"/>
@@ -12464,7 +12764,7 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" ht="12.75" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="10"/>
@@ -12483,7 +12783,7 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
     </row>
-    <row r="71" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" ht="12.75" customHeight="1">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="10"/>
@@ -12502,7 +12802,7 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
     </row>
-    <row r="72" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" ht="12.75" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="10"/>
@@ -12521,7 +12821,7 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" ht="12.75" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="10"/>
@@ -12540,7 +12840,7 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" ht="12.75" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -12559,7 +12859,7 @@
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
     </row>
-    <row r="75" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" ht="12.75" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -12578,7 +12878,7 @@
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
     </row>
-    <row r="76" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" ht="12.75" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="2" t="s">
         <v>329</v>
@@ -12599,7 +12899,7 @@
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
     </row>
-    <row r="77" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" ht="12.75" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="10"/>
@@ -12618,7 +12918,7 @@
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
     </row>
-    <row r="78" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" ht="12.75" customHeight="1">
       <c r="A78" s="1"/>
       <c r="B78" s="1" t="s">
         <v>330</v>
@@ -12639,7 +12939,7 @@
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
     </row>
-    <row r="79" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" ht="12.75" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
         <v>331</v>
@@ -12660,7 +12960,7 @@
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
     </row>
-    <row r="80" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" ht="12.75" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="18" t="str">
         <f>D35</f>
@@ -12682,7 +12982,7 @@
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
     </row>
-    <row r="81" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" ht="12.75" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
         <v>332</v>
@@ -12703,7 +13003,7 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
     </row>
-    <row r="82" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" ht="12.75" customHeight="1">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="10"/>
@@ -12726,6 +13026,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -12737,21 +13042,21 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="3" width="95.85546875" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
-    <col min="9" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" customWidth="1"/>
+    <col min="3" max="3" width="95.83203125" customWidth="1"/>
+    <col min="4" max="4" width="43.5" customWidth="1"/>
+    <col min="5" max="5" width="32.5" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="16" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -12770,7 +13075,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="23.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>333</v>
@@ -12793,7 +13098,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="20" t="str">
         <f>'Iteration 1'!B3</f>
@@ -12815,7 +13120,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="23.25" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="str">
         <f>'Iteration 1'!B5</f>
@@ -12840,7 +13145,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="23.25" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="str">
         <f>'Iteration 1'!B6</f>
@@ -12865,7 +13170,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="22.5" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="str">
         <f>'Iteration 1'!B7</f>
@@ -12890,7 +13195,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="15" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -12909,7 +13214,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="12.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="5" t="s">
         <v>335</v>
@@ -12930,7 +13235,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="13.5" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -12949,7 +13254,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="16.5" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="39" t="s">
         <v>336</v>
@@ -12980,7 +13285,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="7" t="s">
         <v>342</v>
@@ -13008,7 +13313,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="15" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="s">
@@ -13034,7 +13339,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="17.25" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="s">
@@ -13058,7 +13363,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="15" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="s">
@@ -13082,7 +13387,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="15" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
@@ -13108,7 +13413,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
@@ -13132,7 +13437,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="40" t="s">
         <v>352</v>
@@ -13160,7 +13465,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="40"/>
       <c r="C18" s="8" t="s">
@@ -13184,7 +13489,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="40"/>
       <c r="C19" s="8" t="s">
@@ -13209,7 +13514,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="40"/>
       <c r="C20" s="30" t="s">
@@ -13233,7 +13538,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="15" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="40" t="s">
         <v>360</v>
@@ -13261,7 +13566,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="15" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="40"/>
       <c r="C22" s="30" t="s">
@@ -13285,7 +13590,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="15" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="40" t="s">
         <v>364</v>
@@ -13312,7 +13617,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="42" t="s">
         <v>368</v>
@@ -13337,7 +13642,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="13.5" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -13360,5 +13665,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>